<commit_message>
Performer: 6.2.4 Alternative Workflow für Fehler in Workflow 6.2.8 erstellt
</commit_message>
<xml_diff>
--- a/Medavis_Performer_Lunatec/Data/Config.xlsx
+++ b/Medavis_Performer_Lunatec/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas.jahl\develop\RPA\uipath-rpa_med\Medavis_Performer_Lunatec\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas.jahl\develop\uipath\uipath-rpa_med\Medavis_Performer_Lunatec\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EA64AF-8E74-40C2-9582-82F9E5437684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A39A8E9-9A49-4296-9D47-F4B072A65631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1747,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3003,7 +3003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>